<commit_message>
mad and optional stuff
</commit_message>
<xml_diff>
--- a/questionnaires/RBDstandardized_questionnaire_optionalresilience.xlsx
+++ b/questionnaires/RBDstandardized_questionnaire_optionalresilience.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\RBD_Resilience_guide_FR\questionnaires\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A1AE484-52F9-4550-88DD-D8C48EEBC38D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E7F8508-B12E-486F-8C31-1C134F2F034A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="624" uniqueCount="368">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="616" uniqueCount="365">
   <si>
     <t>type</t>
   </si>
@@ -124,12 +124,6 @@
     <t>Je ne sais pas</t>
   </si>
   <si>
-    <t>select_one FIESOuiNon</t>
-  </si>
-  <si>
-    <t>FIESOuiNon</t>
-  </si>
-  <si>
     <t>Services_financiers</t>
   </si>
   <si>
@@ -154,9 +148,6 @@
     <t>Ne sait pas</t>
   </si>
   <si>
-    <t>OuiNonNspRefus</t>
-  </si>
-  <si>
     <t>select_one OuiNonNspRefus</t>
   </si>
   <si>
@@ -178,9 +169,6 @@
     <t>Culture</t>
   </si>
   <si>
-    <t>select_multiple typeAssusrance or_other</t>
-  </si>
-  <si>
     <t>Startegies_Adaption_moyenExist</t>
   </si>
   <si>
@@ -241,12 +229,6 @@
     <t>Expositionchocs5ans</t>
   </si>
   <si>
-    <t>OuiNon</t>
-  </si>
-  <si>
-    <t>select_one OuiNon</t>
-  </si>
-  <si>
     <t>GraviteImpactRevenus</t>
   </si>
   <si>
@@ -304,9 +286,6 @@
     <t>capaciteprofCom</t>
   </si>
   <si>
-    <t>ConnaisAccesUtilisatInfoMarcheIntrant</t>
-  </si>
-  <si>
     <t>Social Capital Index</t>
   </si>
   <si>
@@ -397,18 +376,9 @@
     <t>typedeGroupe</t>
   </si>
   <si>
-    <t>ExistenceGroupeUtilisateurPaturage</t>
-  </si>
-  <si>
     <t>ExistenceGroupeUsagerEau</t>
   </si>
   <si>
-    <t>ExistenceGrouperessourcesNaturelles</t>
-  </si>
-  <si>
-    <t>ExistenceGroupecreditMicrofinance</t>
-  </si>
-  <si>
     <t>ExistenceGroupeEpargne</t>
   </si>
   <si>
@@ -457,15 +427,9 @@
     <t>select_one FrequenceAssistance</t>
   </si>
   <si>
-    <t>FairePartieGroupeAyantfourniNourriture</t>
-  </si>
-  <si>
     <t>FairePartieGroupeAyantfourniAutreAssistance</t>
   </si>
   <si>
-    <t>FairePartieGroupeAyantfourniTravail</t>
-  </si>
-  <si>
     <t xml:space="preserve">Comment appréciez-vous vos capacités à interpeller les dirigeants et les personnes influentes dans cette communité sur certaines questions que vous voulez discuter avec eux ? </t>
   </si>
   <si>
@@ -742,12 +706,6 @@
     <t>RetablissementCapacitesAlim</t>
   </si>
   <si>
-    <t>RetablissementCapacitealimDans1an</t>
-  </si>
-  <si>
-    <t>ConnaisAccesUtilisationInfoMarche</t>
-  </si>
-  <si>
     <t>Est-ce que vous ou quelqu'un d'autre dans votre foyer connaît personnellement un élu du gouvernement ?</t>
   </si>
   <si>
@@ -764,9 +722,6 @@
   </si>
   <si>
     <t>PeutRebombir</t>
-  </si>
-  <si>
-    <t>CapitalisationExperienceAnterieure</t>
   </si>
   <si>
     <t>integer</t>
@@ -1511,10 +1466,46 @@
     <t>Transfertssociaux</t>
   </si>
   <si>
-    <t>OuiNonNsp</t>
-  </si>
-  <si>
     <t>FIESCraintesManquerNourriture</t>
+  </si>
+  <si>
+    <t>Yesnodk</t>
+  </si>
+  <si>
+    <t>Yesnodkref</t>
+  </si>
+  <si>
+    <t>select_one Yesnodkref</t>
+  </si>
+  <si>
+    <t>select_one Yesno</t>
+  </si>
+  <si>
+    <t>RetablissementCapacitealim1an</t>
+  </si>
+  <si>
+    <t>ConAccUtilisationInfoMarche</t>
+  </si>
+  <si>
+    <t>ConAccUtilisatInfoMarcheIntrant</t>
+  </si>
+  <si>
+    <t>ExistenceGroupecreditMicrofinan</t>
+  </si>
+  <si>
+    <t>ExistenceGroupeUtilisateurPat</t>
+  </si>
+  <si>
+    <t>ExistenceGrouperessourcesNat</t>
+  </si>
+  <si>
+    <t>FairePartieGroupeAyantfouTrav</t>
+  </si>
+  <si>
+    <t>FairePartieGroupeAyantfouNour</t>
+  </si>
+  <si>
+    <t>CapitalisationExperienceAnt</t>
   </si>
 </sst>
 </file>
@@ -1723,7 +1714,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -1826,7 +1817,19 @@
     <xf numFmtId="0" fontId="17" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2143,14 +2146,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N114"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A94" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" topLeftCell="A103" workbookViewId="0">
+      <selection activeCell="A114" sqref="A114"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="21.5703125" style="33" customWidth="1"/>
-    <col min="2" max="2" width="25.28515625" style="33" customWidth="1"/>
+    <col min="2" max="2" width="33.28515625" style="44" customWidth="1"/>
     <col min="3" max="3" width="65.7109375" style="9" customWidth="1"/>
     <col min="4" max="4" width="67.5703125" style="9" customWidth="1"/>
     <col min="5" max="16384" width="9.140625" style="9"/>
@@ -2160,7 +2163,7 @@
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="43" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="6" t="s">
@@ -2200,7 +2203,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="24" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:14" s="12" customFormat="1" ht="24" x14ac:dyDescent="0.2">
       <c r="A2" s="32" t="s">
         <v>19</v>
       </c>
@@ -2208,130 +2211,119 @@
         <v>20</v>
       </c>
       <c r="C2" s="18" t="s">
-        <v>249</v>
-      </c>
-      <c r="D2" s="12"/>
-      <c r="E2" s="12"/>
-      <c r="F2" s="12"/>
-      <c r="G2" s="12"/>
-      <c r="H2" s="12"/>
-      <c r="I2" s="12"/>
-      <c r="J2" s="12"/>
-      <c r="K2" s="12"/>
-      <c r="L2" s="12"/>
-      <c r="M2" s="12"/>
-      <c r="N2" s="12"/>
+        <v>234</v>
+      </c>
     </row>
     <row r="3" spans="1:14" ht="55.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="33" t="s">
-        <v>29</v>
-      </c>
-      <c r="B3" s="42" t="s">
-        <v>367</v>
+        <v>354</v>
+      </c>
+      <c r="B3" s="45" t="s">
+        <v>351</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>248</v>
+        <v>233</v>
       </c>
       <c r="G3" s="9" t="s">
-        <v>333</v>
+        <v>318</v>
       </c>
     </row>
     <row r="4" spans="1:14" ht="48" x14ac:dyDescent="0.2">
       <c r="A4" s="33" t="s">
-        <v>29</v>
-      </c>
-      <c r="B4" s="33" t="s">
-        <v>177</v>
+        <v>354</v>
+      </c>
+      <c r="B4" s="44" t="s">
+        <v>165</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>247</v>
+        <v>232</v>
       </c>
       <c r="G4" s="9" t="s">
-        <v>333</v>
+        <v>318</v>
       </c>
     </row>
     <row r="5" spans="1:14" ht="48" x14ac:dyDescent="0.2">
       <c r="A5" s="33" t="s">
-        <v>29</v>
-      </c>
-      <c r="B5" s="33" t="s">
+        <v>354</v>
+      </c>
+      <c r="B5" s="44" t="s">
         <v>24</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>250</v>
+        <v>235</v>
       </c>
       <c r="G5" s="9" t="s">
-        <v>333</v>
+        <v>318</v>
       </c>
     </row>
     <row r="6" spans="1:14" ht="48" x14ac:dyDescent="0.2">
       <c r="A6" s="33" t="s">
-        <v>29</v>
-      </c>
-      <c r="B6" s="33" t="s">
-        <v>175</v>
+        <v>354</v>
+      </c>
+      <c r="B6" s="44" t="s">
+        <v>163</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>251</v>
+        <v>236</v>
       </c>
       <c r="G6" s="9" t="s">
-        <v>333</v>
+        <v>318</v>
       </c>
     </row>
     <row r="7" spans="1:14" ht="48" x14ac:dyDescent="0.2">
       <c r="A7" s="33" t="s">
-        <v>29</v>
-      </c>
-      <c r="B7" s="33" t="s">
-        <v>176</v>
+        <v>354</v>
+      </c>
+      <c r="B7" s="44" t="s">
+        <v>164</v>
       </c>
       <c r="C7" s="10" t="s">
-        <v>252</v>
+        <v>237</v>
       </c>
       <c r="G7" s="9" t="s">
-        <v>333</v>
+        <v>318</v>
       </c>
     </row>
     <row r="8" spans="1:14" ht="36" x14ac:dyDescent="0.2">
       <c r="A8" s="33" t="s">
-        <v>29</v>
-      </c>
-      <c r="B8" s="33" t="s">
+        <v>354</v>
+      </c>
+      <c r="B8" s="44" t="s">
         <v>21</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>253</v>
+        <v>238</v>
       </c>
       <c r="G8" s="9" t="s">
-        <v>333</v>
+        <v>318</v>
       </c>
     </row>
     <row r="9" spans="1:14" ht="48" x14ac:dyDescent="0.2">
       <c r="A9" s="33" t="s">
-        <v>29</v>
-      </c>
-      <c r="B9" s="33" t="s">
+        <v>354</v>
+      </c>
+      <c r="B9" s="44" t="s">
         <v>22</v>
       </c>
       <c r="C9" s="10" t="s">
-        <v>254</v>
+        <v>239</v>
       </c>
       <c r="G9" s="9" t="s">
-        <v>333</v>
+        <v>318</v>
       </c>
     </row>
     <row r="10" spans="1:14" ht="48" x14ac:dyDescent="0.2">
       <c r="A10" s="33" t="s">
-        <v>29</v>
-      </c>
-      <c r="B10" s="33" t="s">
+        <v>354</v>
+      </c>
+      <c r="B10" s="44" t="s">
         <v>23</v>
       </c>
       <c r="C10" s="10" t="s">
-        <v>255</v>
+        <v>240</v>
       </c>
       <c r="G10" s="9" t="s">
-        <v>333</v>
+        <v>318</v>
       </c>
     </row>
     <row r="11" spans="1:14" s="12" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
@@ -2339,77 +2331,77 @@
         <v>19</v>
       </c>
       <c r="B11" s="34" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C11" s="20" t="s">
-        <v>256</v>
+        <v>241</v>
       </c>
     </row>
     <row r="12" spans="1:14" ht="24" x14ac:dyDescent="0.2">
       <c r="A12" s="33" t="s">
-        <v>40</v>
-      </c>
-      <c r="B12" s="33" t="s">
-        <v>35</v>
+        <v>354</v>
+      </c>
+      <c r="B12" s="44" t="s">
+        <v>33</v>
       </c>
       <c r="C12" s="10" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="G12" s="9" t="s">
-        <v>333</v>
+        <v>318</v>
       </c>
     </row>
     <row r="13" spans="1:14" ht="24" x14ac:dyDescent="0.2">
       <c r="A13" s="33" t="s">
-        <v>40</v>
-      </c>
-      <c r="B13" s="33" t="s">
-        <v>179</v>
+        <v>354</v>
+      </c>
+      <c r="B13" s="44" t="s">
+        <v>167</v>
       </c>
       <c r="C13" s="10" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="G13" s="9" t="s">
-        <v>333</v>
+        <v>318</v>
       </c>
     </row>
     <row r="14" spans="1:14" ht="24" x14ac:dyDescent="0.2">
       <c r="A14" s="33" t="s">
-        <v>40</v>
-      </c>
-      <c r="B14" s="33" t="s">
-        <v>36</v>
+        <v>354</v>
+      </c>
+      <c r="B14" s="44" t="s">
+        <v>34</v>
       </c>
       <c r="C14" s="10" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="G14" s="9" t="s">
-        <v>333</v>
+        <v>318</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A15" s="33" t="s">
-        <v>40</v>
-      </c>
-      <c r="B15" s="33" t="s">
-        <v>180</v>
+        <v>354</v>
+      </c>
+      <c r="B15" s="44" t="s">
+        <v>168</v>
       </c>
       <c r="C15" s="10" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="G15" s="9" t="s">
-        <v>333</v>
+        <v>318</v>
       </c>
     </row>
     <row r="16" spans="1:14" ht="24" x14ac:dyDescent="0.2">
       <c r="A16" s="33" t="s">
-        <v>47</v>
-      </c>
-      <c r="B16" s="33" t="s">
-        <v>44</v>
+        <v>354</v>
+      </c>
+      <c r="B16" s="44" t="s">
+        <v>41</v>
       </c>
       <c r="C16" s="10" t="s">
-        <v>245</v>
+        <v>230</v>
       </c>
     </row>
     <row r="18" spans="1:8" s="19" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2417,10 +2409,10 @@
         <v>19</v>
       </c>
       <c r="B18" s="34" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="C18" s="20" t="s">
-        <v>257</v>
+        <v>242</v>
       </c>
     </row>
     <row r="19" spans="1:8" s="19" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -2428,551 +2420,551 @@
         <v>19</v>
       </c>
       <c r="B19" s="34" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="C19" s="20" t="s">
-        <v>258</v>
+        <v>243</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20" s="33" t="s">
-        <v>64</v>
-      </c>
-      <c r="B20" s="33" t="s">
-        <v>185</v>
+        <v>60</v>
+      </c>
+      <c r="B20" s="44" t="s">
+        <v>173</v>
       </c>
       <c r="C20" s="13"/>
       <c r="H20" s="9" t="s">
-        <v>178</v>
+        <v>166</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21" s="33" t="s">
+        <v>229</v>
+      </c>
+      <c r="B21" s="44" t="s">
+        <v>172</v>
+      </c>
+      <c r="C21" s="13" t="s">
         <v>244</v>
       </c>
-      <c r="B21" s="33" t="s">
-        <v>184</v>
-      </c>
-      <c r="C21" s="13" t="s">
-        <v>259</v>
-      </c>
       <c r="G21" s="9" t="s">
-        <v>333</v>
+        <v>318</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22" s="33" t="s">
-        <v>244</v>
-      </c>
-      <c r="B22" s="33" t="s">
-        <v>183</v>
+        <v>229</v>
+      </c>
+      <c r="B22" s="44" t="s">
+        <v>171</v>
       </c>
       <c r="C22" s="13" t="s">
-        <v>260</v>
+        <v>245</v>
       </c>
       <c r="G22" s="9" t="s">
-        <v>333</v>
+        <v>318</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23" s="33" t="s">
-        <v>244</v>
-      </c>
-      <c r="B23" s="33" t="s">
-        <v>182</v>
+        <v>229</v>
+      </c>
+      <c r="B23" s="44" t="s">
+        <v>170</v>
       </c>
       <c r="C23" s="13" t="s">
-        <v>261</v>
+        <v>246</v>
       </c>
       <c r="G23" s="9" t="s">
-        <v>333</v>
+        <v>318</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A24" s="33" t="s">
-        <v>244</v>
-      </c>
-      <c r="B24" s="33" t="s">
-        <v>186</v>
+        <v>229</v>
+      </c>
+      <c r="B24" s="44" t="s">
+        <v>174</v>
       </c>
       <c r="C24" s="13" t="s">
-        <v>262</v>
+        <v>247</v>
       </c>
       <c r="G24" s="9" t="s">
-        <v>333</v>
+        <v>318</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A25" s="33" t="s">
-        <v>244</v>
-      </c>
-      <c r="B25" s="33" t="s">
-        <v>187</v>
+        <v>229</v>
+      </c>
+      <c r="B25" s="44" t="s">
+        <v>175</v>
       </c>
       <c r="C25" s="13" t="s">
-        <v>263</v>
+        <v>248</v>
       </c>
       <c r="G25" s="9" t="s">
-        <v>333</v>
+        <v>318</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A26" s="33" t="s">
-        <v>244</v>
-      </c>
-      <c r="B26" s="33" t="s">
-        <v>188</v>
+        <v>229</v>
+      </c>
+      <c r="B26" s="44" t="s">
+        <v>176</v>
       </c>
       <c r="C26" s="13" t="s">
-        <v>264</v>
+        <v>249</v>
       </c>
       <c r="G26" s="9" t="s">
-        <v>333</v>
+        <v>318</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A27" s="33" t="s">
-        <v>244</v>
-      </c>
-      <c r="B27" s="33" t="s">
-        <v>189</v>
+        <v>229</v>
+      </c>
+      <c r="B27" s="44" t="s">
+        <v>177</v>
       </c>
       <c r="C27" s="13" t="s">
-        <v>265</v>
+        <v>250</v>
       </c>
       <c r="G27" s="9" t="s">
-        <v>333</v>
+        <v>318</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A28" s="33" t="s">
-        <v>244</v>
-      </c>
-      <c r="B28" s="33" t="s">
-        <v>190</v>
+        <v>229</v>
+      </c>
+      <c r="B28" s="44" t="s">
+        <v>178</v>
       </c>
       <c r="C28" s="13" t="s">
-        <v>266</v>
+        <v>251</v>
       </c>
       <c r="G28" s="9" t="s">
-        <v>333</v>
+        <v>318</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A29" s="33" t="s">
-        <v>244</v>
-      </c>
-      <c r="B29" s="33" t="s">
-        <v>191</v>
+        <v>229</v>
+      </c>
+      <c r="B29" s="44" t="s">
+        <v>179</v>
       </c>
       <c r="C29" s="13" t="s">
-        <v>267</v>
+        <v>252</v>
       </c>
       <c r="G29" s="9" t="s">
-        <v>333</v>
+        <v>318</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A30" s="33" t="s">
-        <v>244</v>
-      </c>
-      <c r="B30" s="33" t="s">
-        <v>192</v>
+        <v>229</v>
+      </c>
+      <c r="B30" s="44" t="s">
+        <v>180</v>
       </c>
       <c r="C30" s="13" t="s">
-        <v>268</v>
+        <v>253</v>
       </c>
       <c r="G30" s="9" t="s">
-        <v>333</v>
+        <v>318</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A31" s="33" t="s">
-        <v>244</v>
-      </c>
-      <c r="B31" s="33" t="s">
-        <v>193</v>
+        <v>229</v>
+      </c>
+      <c r="B31" s="44" t="s">
+        <v>181</v>
       </c>
       <c r="C31" s="13" t="s">
-        <v>269</v>
+        <v>254</v>
       </c>
       <c r="G31" s="9" t="s">
-        <v>333</v>
+        <v>318</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A32" s="33" t="s">
-        <v>244</v>
-      </c>
-      <c r="B32" s="33" t="s">
-        <v>194</v>
+        <v>229</v>
+      </c>
+      <c r="B32" s="44" t="s">
+        <v>182</v>
       </c>
       <c r="C32" s="13" t="s">
-        <v>270</v>
+        <v>255</v>
       </c>
       <c r="G32" s="9" t="s">
-        <v>333</v>
+        <v>318</v>
       </c>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A33" s="33" t="s">
-        <v>244</v>
-      </c>
-      <c r="B33" s="33" t="s">
-        <v>195</v>
+        <v>229</v>
+      </c>
+      <c r="B33" s="44" t="s">
+        <v>183</v>
       </c>
       <c r="C33" s="13" t="s">
-        <v>271</v>
+        <v>256</v>
       </c>
       <c r="G33" s="9" t="s">
-        <v>333</v>
+        <v>318</v>
       </c>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A34" s="33" t="s">
-        <v>244</v>
-      </c>
-      <c r="B34" s="33" t="s">
-        <v>196</v>
+        <v>229</v>
+      </c>
+      <c r="B34" s="44" t="s">
+        <v>184</v>
       </c>
       <c r="C34" s="13" t="s">
-        <v>272</v>
+        <v>257</v>
       </c>
       <c r="G34" s="9" t="s">
-        <v>333</v>
+        <v>318</v>
       </c>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A35" s="33" t="s">
-        <v>244</v>
-      </c>
-      <c r="B35" s="33" t="s">
-        <v>197</v>
+        <v>229</v>
+      </c>
+      <c r="B35" s="44" t="s">
+        <v>185</v>
       </c>
       <c r="C35" s="13" t="s">
-        <v>273</v>
+        <v>258</v>
       </c>
       <c r="G35" s="9" t="s">
-        <v>333</v>
+        <v>318</v>
       </c>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A36" s="33" t="s">
-        <v>244</v>
-      </c>
-      <c r="B36" s="33" t="s">
-        <v>198</v>
+        <v>229</v>
+      </c>
+      <c r="B36" s="44" t="s">
+        <v>186</v>
       </c>
       <c r="C36" s="13" t="s">
-        <v>274</v>
+        <v>259</v>
       </c>
       <c r="G36" s="9" t="s">
-        <v>333</v>
+        <v>318</v>
       </c>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A37" s="33" t="s">
-        <v>244</v>
-      </c>
-      <c r="B37" s="33" t="s">
-        <v>199</v>
+        <v>229</v>
+      </c>
+      <c r="B37" s="44" t="s">
+        <v>187</v>
       </c>
       <c r="C37" s="14" t="s">
-        <v>275</v>
+        <v>260</v>
       </c>
       <c r="G37" s="9" t="s">
-        <v>333</v>
+        <v>318</v>
       </c>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A38" s="33" t="s">
-        <v>132</v>
+        <v>122</v>
       </c>
       <c r="C38" s="14"/>
     </row>
     <row r="39" spans="1:10" ht="24" x14ac:dyDescent="0.2">
       <c r="A39" s="33" t="s">
-        <v>64</v>
-      </c>
-      <c r="B39" s="33" t="s">
-        <v>346</v>
+        <v>60</v>
+      </c>
+      <c r="B39" s="44" t="s">
+        <v>331</v>
       </c>
       <c r="C39" s="15" t="s">
-        <v>181</v>
+        <v>169</v>
       </c>
       <c r="H39" s="9" t="s">
-        <v>178</v>
+        <v>166</v>
       </c>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A40" s="33" t="s">
-        <v>69</v>
-      </c>
-      <c r="B40" s="33" t="s">
-        <v>218</v>
+        <v>355</v>
+      </c>
+      <c r="B40" s="44" t="s">
+        <v>206</v>
       </c>
       <c r="C40" s="13" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="J40" s="9" t="s">
-        <v>200</v>
+        <v>188</v>
       </c>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A41" s="33" t="s">
-        <v>69</v>
-      </c>
-      <c r="B41" s="33" t="s">
-        <v>217</v>
+        <v>355</v>
+      </c>
+      <c r="B41" s="44" t="s">
+        <v>205</v>
       </c>
       <c r="C41" s="13" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="J41" s="9" t="s">
-        <v>201</v>
+        <v>189</v>
       </c>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A42" s="33" t="s">
-        <v>69</v>
-      </c>
-      <c r="B42" s="33" t="s">
-        <v>219</v>
+        <v>355</v>
+      </c>
+      <c r="B42" s="44" t="s">
+        <v>207</v>
       </c>
       <c r="C42" s="13" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="J42" s="9" t="s">
-        <v>202</v>
+        <v>190</v>
       </c>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A43" s="33" t="s">
-        <v>69</v>
-      </c>
-      <c r="B43" s="33" t="s">
-        <v>220</v>
+        <v>355</v>
+      </c>
+      <c r="B43" s="44" t="s">
+        <v>208</v>
       </c>
       <c r="C43" s="13" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="J43" s="9" t="s">
-        <v>203</v>
+        <v>191</v>
       </c>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A44" s="33" t="s">
-        <v>69</v>
-      </c>
-      <c r="B44" s="33" t="s">
-        <v>221</v>
+        <v>355</v>
+      </c>
+      <c r="B44" s="44" t="s">
+        <v>209</v>
       </c>
       <c r="C44" s="13" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="J44" s="9" t="s">
-        <v>204</v>
+        <v>192</v>
       </c>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A45" s="33" t="s">
-        <v>69</v>
-      </c>
-      <c r="B45" s="33" t="s">
-        <v>222</v>
+        <v>355</v>
+      </c>
+      <c r="B45" s="44" t="s">
+        <v>210</v>
       </c>
       <c r="C45" s="13" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="J45" s="9" t="s">
-        <v>205</v>
+        <v>193</v>
       </c>
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A46" s="33" t="s">
-        <v>69</v>
-      </c>
-      <c r="B46" s="33" t="s">
-        <v>223</v>
+        <v>355</v>
+      </c>
+      <c r="B46" s="44" t="s">
+        <v>211</v>
       </c>
       <c r="C46" s="13" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="J46" s="9" t="s">
-        <v>206</v>
+        <v>194</v>
       </c>
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A47" s="33" t="s">
-        <v>69</v>
-      </c>
-      <c r="B47" s="33" t="s">
-        <v>224</v>
+        <v>355</v>
+      </c>
+      <c r="B47" s="44" t="s">
+        <v>212</v>
       </c>
       <c r="C47" s="13" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="J47" s="9" t="s">
-        <v>207</v>
+        <v>195</v>
       </c>
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A48" s="33" t="s">
-        <v>69</v>
-      </c>
-      <c r="B48" s="33" t="s">
-        <v>225</v>
+        <v>355</v>
+      </c>
+      <c r="B48" s="44" t="s">
+        <v>213</v>
       </c>
       <c r="C48" s="13" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="J48" s="9" t="s">
-        <v>208</v>
+        <v>196</v>
       </c>
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A49" s="33" t="s">
-        <v>69</v>
-      </c>
-      <c r="B49" s="33" t="s">
-        <v>226</v>
+        <v>355</v>
+      </c>
+      <c r="B49" s="44" t="s">
+        <v>214</v>
       </c>
       <c r="C49" s="13" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="J49" s="9" t="s">
-        <v>209</v>
+        <v>197</v>
       </c>
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A50" s="33" t="s">
-        <v>69</v>
-      </c>
-      <c r="B50" s="33" t="s">
-        <v>227</v>
+        <v>355</v>
+      </c>
+      <c r="B50" s="44" t="s">
+        <v>215</v>
       </c>
       <c r="C50" s="13" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="J50" s="9" t="s">
-        <v>210</v>
+        <v>198</v>
       </c>
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A51" s="33" t="s">
-        <v>69</v>
-      </c>
-      <c r="B51" s="33" t="s">
-        <v>228</v>
+        <v>355</v>
+      </c>
+      <c r="B51" s="44" t="s">
+        <v>216</v>
       </c>
       <c r="C51" s="13" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="J51" s="9" t="s">
-        <v>211</v>
+        <v>199</v>
       </c>
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A52" s="33" t="s">
-        <v>69</v>
-      </c>
-      <c r="B52" s="33" t="s">
-        <v>229</v>
+        <v>355</v>
+      </c>
+      <c r="B52" s="44" t="s">
+        <v>217</v>
       </c>
       <c r="C52" s="13" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="J52" s="9" t="s">
-        <v>212</v>
+        <v>200</v>
       </c>
     </row>
     <row r="53" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A53" s="33" t="s">
-        <v>69</v>
-      </c>
-      <c r="B53" s="33" t="s">
-        <v>230</v>
+        <v>355</v>
+      </c>
+      <c r="B53" s="44" t="s">
+        <v>218</v>
       </c>
       <c r="C53" s="13" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="J53" s="9" t="s">
-        <v>213</v>
+        <v>201</v>
       </c>
     </row>
     <row r="54" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A54" s="33" t="s">
-        <v>69</v>
-      </c>
-      <c r="B54" s="33" t="s">
-        <v>231</v>
+        <v>355</v>
+      </c>
+      <c r="B54" s="44" t="s">
+        <v>219</v>
       </c>
       <c r="C54" s="13" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="J54" s="9" t="s">
-        <v>214</v>
+        <v>202</v>
       </c>
     </row>
     <row r="55" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A55" s="33" t="s">
-        <v>69</v>
-      </c>
-      <c r="B55" s="33" t="s">
-        <v>232</v>
+        <v>355</v>
+      </c>
+      <c r="B55" s="44" t="s">
+        <v>220</v>
       </c>
       <c r="C55" s="13" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="J55" s="9" t="s">
-        <v>215</v>
+        <v>203</v>
       </c>
     </row>
     <row r="56" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A56" s="33" t="s">
-        <v>69</v>
-      </c>
-      <c r="B56" s="33" t="s">
-        <v>233</v>
+        <v>355</v>
+      </c>
+      <c r="B56" s="44" t="s">
+        <v>221</v>
       </c>
       <c r="C56" s="14" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="J56" s="9" t="s">
-        <v>216</v>
+        <v>204</v>
       </c>
     </row>
     <row r="57" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A57" s="33" t="s">
-        <v>132</v>
+        <v>122</v>
       </c>
     </row>
     <row r="58" spans="1:10" ht="24" x14ac:dyDescent="0.2">
       <c r="A58" s="33" t="s">
-        <v>78</v>
-      </c>
-      <c r="B58" s="33" t="s">
-        <v>70</v>
+        <v>72</v>
+      </c>
+      <c r="B58" s="44" t="s">
+        <v>64</v>
       </c>
       <c r="C58" s="15" t="s">
-        <v>334</v>
+        <v>319</v>
       </c>
       <c r="H58" s="9" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
     </row>
     <row r="59" spans="1:10" ht="36" x14ac:dyDescent="0.2">
       <c r="A59" s="33" t="s">
-        <v>78</v>
-      </c>
-      <c r="B59" s="33" t="s">
-        <v>79</v>
+        <v>72</v>
+      </c>
+      <c r="B59" s="44" t="s">
+        <v>73</v>
       </c>
       <c r="C59" s="15" t="s">
-        <v>335</v>
+        <v>320</v>
       </c>
       <c r="H59" s="9" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
     </row>
     <row r="60" spans="1:10" s="19" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -2980,91 +2972,91 @@
         <v>19</v>
       </c>
       <c r="B60" s="34" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="C60" s="22" t="s">
-        <v>276</v>
+        <v>261</v>
       </c>
     </row>
     <row r="61" spans="1:10" customFormat="1" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="33" t="s">
-        <v>345</v>
-      </c>
-      <c r="B61" s="33" t="s">
-        <v>336</v>
+        <v>330</v>
+      </c>
+      <c r="B61" s="44" t="s">
+        <v>321</v>
       </c>
       <c r="C61" s="31" t="s">
-        <v>338</v>
+        <v>323</v>
       </c>
     </row>
     <row r="62" spans="1:10" ht="48" x14ac:dyDescent="0.2">
       <c r="A62" s="33" t="s">
-        <v>86</v>
-      </c>
-      <c r="B62" s="33" t="s">
-        <v>234</v>
+        <v>80</v>
+      </c>
+      <c r="B62" s="44" t="s">
+        <v>222</v>
       </c>
       <c r="C62" s="16" t="s">
-        <v>278</v>
+        <v>263</v>
       </c>
       <c r="G62" s="9" t="s">
-        <v>333</v>
+        <v>318</v>
       </c>
     </row>
     <row r="63" spans="1:10" ht="36" x14ac:dyDescent="0.2">
       <c r="A63" s="33" t="s">
-        <v>86</v>
-      </c>
-      <c r="B63" s="33" t="s">
-        <v>235</v>
+        <v>80</v>
+      </c>
+      <c r="B63" s="44" t="s">
+        <v>356</v>
       </c>
       <c r="C63" s="16" t="s">
-        <v>277</v>
+        <v>262</v>
       </c>
       <c r="G63" s="9" t="s">
-        <v>333</v>
+        <v>318</v>
       </c>
     </row>
     <row r="64" spans="1:10" ht="36" x14ac:dyDescent="0.2">
       <c r="A64" s="33" t="s">
-        <v>69</v>
-      </c>
-      <c r="B64" s="33" t="s">
-        <v>88</v>
+        <v>355</v>
+      </c>
+      <c r="B64" s="44" t="s">
+        <v>82</v>
       </c>
       <c r="C64" s="16" t="s">
-        <v>279</v>
+        <v>264</v>
       </c>
       <c r="G64" s="9" t="s">
-        <v>333</v>
+        <v>318</v>
       </c>
     </row>
     <row r="65" spans="1:8" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A65" s="33" t="s">
-        <v>69</v>
-      </c>
-      <c r="B65" s="33" t="s">
-        <v>89</v>
+        <v>355</v>
+      </c>
+      <c r="B65" s="44" t="s">
+        <v>358</v>
       </c>
       <c r="C65" s="30" t="s">
-        <v>280</v>
+        <v>265</v>
       </c>
       <c r="G65" s="9" t="s">
-        <v>333</v>
+        <v>318</v>
       </c>
     </row>
     <row r="66" spans="1:8" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A66" s="33" t="s">
-        <v>69</v>
-      </c>
-      <c r="B66" s="33" t="s">
-        <v>236</v>
+        <v>355</v>
+      </c>
+      <c r="B66" s="44" t="s">
+        <v>357</v>
       </c>
       <c r="C66" s="16" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="G66" s="9" t="s">
-        <v>333</v>
+        <v>318</v>
       </c>
     </row>
     <row r="67" spans="1:8" s="19" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -3072,164 +3064,164 @@
         <v>19</v>
       </c>
       <c r="B67" s="35" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
       <c r="C67" s="21" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
     </row>
     <row r="68" spans="1:8" ht="60" x14ac:dyDescent="0.2">
       <c r="A68" s="33" t="s">
-        <v>95</v>
-      </c>
-      <c r="B68" s="33" t="s">
-        <v>92</v>
+        <v>88</v>
+      </c>
+      <c r="B68" s="44" t="s">
+        <v>85</v>
       </c>
       <c r="C68" s="16" t="s">
-        <v>282</v>
+        <v>267</v>
       </c>
       <c r="G68" s="9" t="s">
-        <v>333</v>
+        <v>318</v>
       </c>
     </row>
     <row r="69" spans="1:8" ht="48" x14ac:dyDescent="0.2">
       <c r="A69" s="33" t="s">
-        <v>95</v>
-      </c>
-      <c r="B69" s="33" t="s">
-        <v>96</v>
+        <v>88</v>
+      </c>
+      <c r="B69" s="44" t="s">
+        <v>89</v>
       </c>
       <c r="C69" s="16" t="s">
-        <v>281</v>
+        <v>266</v>
       </c>
       <c r="G69" s="9" t="s">
-        <v>333</v>
+        <v>318</v>
       </c>
     </row>
     <row r="70" spans="1:8" ht="24" x14ac:dyDescent="0.2">
       <c r="A70" s="33" t="s">
-        <v>99</v>
-      </c>
-      <c r="B70" s="33" t="s">
-        <v>98</v>
+        <v>92</v>
+      </c>
+      <c r="B70" s="44" t="s">
+        <v>91</v>
       </c>
       <c r="C70" s="16" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
       <c r="G70" s="9" t="s">
-        <v>333</v>
+        <v>318</v>
       </c>
     </row>
     <row r="71" spans="1:8" ht="36" x14ac:dyDescent="0.2">
       <c r="A71" s="33" t="s">
-        <v>95</v>
-      </c>
-      <c r="B71" s="33" t="s">
-        <v>101</v>
+        <v>88</v>
+      </c>
+      <c r="B71" s="44" t="s">
+        <v>94</v>
       </c>
       <c r="C71" s="16" t="s">
-        <v>283</v>
+        <v>268</v>
       </c>
       <c r="G71" s="9" t="s">
-        <v>333</v>
+        <v>318</v>
       </c>
     </row>
     <row r="72" spans="1:8" ht="36" x14ac:dyDescent="0.2">
       <c r="A72" s="33" t="s">
+        <v>88</v>
+      </c>
+      <c r="B72" s="44" t="s">
         <v>95</v>
       </c>
-      <c r="B72" s="33" t="s">
-        <v>102</v>
-      </c>
       <c r="C72" s="16" t="s">
-        <v>284</v>
+        <v>269</v>
       </c>
       <c r="G72" s="9" t="s">
-        <v>333</v>
+        <v>318</v>
       </c>
     </row>
     <row r="73" spans="1:8" ht="24" x14ac:dyDescent="0.2">
       <c r="A73" s="33" t="s">
-        <v>40</v>
-      </c>
-      <c r="B73" s="33" t="s">
-        <v>103</v>
+        <v>37</v>
+      </c>
+      <c r="B73" s="44" t="s">
+        <v>96</v>
       </c>
       <c r="C73" s="16" t="s">
-        <v>237</v>
+        <v>223</v>
       </c>
       <c r="G73" s="9" t="s">
-        <v>333</v>
+        <v>318</v>
       </c>
     </row>
     <row r="74" spans="1:8" ht="36" x14ac:dyDescent="0.2">
       <c r="A74" s="33" t="s">
-        <v>110</v>
-      </c>
-      <c r="B74" s="33" t="s">
-        <v>112</v>
+        <v>103</v>
+      </c>
+      <c r="B74" s="44" t="s">
+        <v>105</v>
       </c>
       <c r="C74" s="16" t="s">
-        <v>238</v>
+        <v>224</v>
       </c>
       <c r="G74" s="9" t="s">
-        <v>333</v>
+        <v>318</v>
       </c>
     </row>
     <row r="75" spans="1:8" ht="24" x14ac:dyDescent="0.2">
       <c r="A75" s="33" t="s">
-        <v>40</v>
-      </c>
-      <c r="B75" s="33" t="s">
-        <v>113</v>
+        <v>37</v>
+      </c>
+      <c r="B75" s="44" t="s">
+        <v>106</v>
       </c>
       <c r="C75" s="16" t="s">
-        <v>239</v>
+        <v>225</v>
       </c>
       <c r="G75" s="9" t="s">
-        <v>333</v>
+        <v>318</v>
       </c>
     </row>
     <row r="76" spans="1:8" ht="36" x14ac:dyDescent="0.2">
       <c r="A76" s="33" t="s">
-        <v>40</v>
-      </c>
-      <c r="B76" s="33" t="s">
-        <v>111</v>
+        <v>37</v>
+      </c>
+      <c r="B76" s="44" t="s">
+        <v>104</v>
       </c>
       <c r="C76" s="16" t="s">
-        <v>285</v>
+        <v>270</v>
       </c>
       <c r="G76" s="9" t="s">
-        <v>333</v>
+        <v>318</v>
       </c>
     </row>
     <row r="77" spans="1:8" ht="24" x14ac:dyDescent="0.2">
       <c r="A77" s="33" t="s">
-        <v>110</v>
-      </c>
-      <c r="B77" s="33" t="s">
-        <v>114</v>
+        <v>103</v>
+      </c>
+      <c r="B77" s="44" t="s">
+        <v>107</v>
       </c>
       <c r="C77" s="16" t="s">
-        <v>240</v>
+        <v>226</v>
       </c>
       <c r="G77" s="9" t="s">
-        <v>333</v>
+        <v>318</v>
       </c>
     </row>
     <row r="78" spans="1:8" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A78" s="33" t="s">
-        <v>40</v>
-      </c>
-      <c r="B78" s="33" t="s">
-        <v>115</v>
+        <v>354</v>
+      </c>
+      <c r="B78" s="44" t="s">
+        <v>108</v>
       </c>
       <c r="C78" s="16" t="s">
-        <v>241</v>
+        <v>227</v>
       </c>
       <c r="G78" s="9" t="s">
-        <v>333</v>
+        <v>318</v>
       </c>
     </row>
     <row r="79" spans="1:8" s="12" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -3237,265 +3229,265 @@
         <v>19</v>
       </c>
       <c r="B79" s="34" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
       <c r="C79" s="21" t="s">
-        <v>116</v>
+        <v>109</v>
       </c>
     </row>
     <row r="80" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A80" s="33" t="s">
-        <v>64</v>
-      </c>
-      <c r="B80" s="33" t="s">
-        <v>118</v>
+        <v>60</v>
+      </c>
+      <c r="B80" s="44" t="s">
+        <v>111</v>
       </c>
       <c r="C80" s="10"/>
       <c r="H80" s="9" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A81" s="33" t="s">
-        <v>40</v>
-      </c>
-      <c r="B81" s="33" t="s">
-        <v>121</v>
+        <v>354</v>
+      </c>
+      <c r="B81" s="44" t="s">
+        <v>113</v>
       </c>
       <c r="C81" s="9" t="s">
-        <v>286</v>
+        <v>271</v>
       </c>
       <c r="G81" s="9" t="s">
-        <v>333</v>
+        <v>318</v>
       </c>
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A82" s="33" t="s">
-        <v>40</v>
-      </c>
-      <c r="B82" s="33" t="s">
-        <v>120</v>
+        <v>354</v>
+      </c>
+      <c r="B82" s="44" t="s">
+        <v>360</v>
       </c>
       <c r="C82" s="9" t="s">
-        <v>287</v>
+        <v>272</v>
       </c>
       <c r="G82" s="9" t="s">
-        <v>333</v>
+        <v>318</v>
       </c>
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A83" s="33" t="s">
-        <v>40</v>
-      </c>
-      <c r="B83" s="33" t="s">
-        <v>122</v>
+        <v>354</v>
+      </c>
+      <c r="B83" s="44" t="s">
+        <v>361</v>
       </c>
       <c r="C83" s="9" t="s">
-        <v>288</v>
+        <v>273</v>
       </c>
       <c r="G83" s="9" t="s">
-        <v>333</v>
+        <v>318</v>
       </c>
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A84" s="33" t="s">
-        <v>40</v>
-      </c>
-      <c r="B84" s="33" t="s">
-        <v>123</v>
+        <v>354</v>
+      </c>
+      <c r="B84" s="44" t="s">
+        <v>359</v>
       </c>
       <c r="C84" s="9" t="s">
-        <v>289</v>
+        <v>274</v>
       </c>
       <c r="G84" s="9" t="s">
-        <v>333</v>
+        <v>318</v>
       </c>
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A85" s="33" t="s">
-        <v>40</v>
-      </c>
-      <c r="B85" s="33" t="s">
-        <v>124</v>
+        <v>354</v>
+      </c>
+      <c r="B85" s="44" t="s">
+        <v>114</v>
       </c>
       <c r="C85" s="9" t="s">
-        <v>290</v>
+        <v>275</v>
       </c>
       <c r="G85" s="9" t="s">
-        <v>333</v>
+        <v>318</v>
       </c>
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A86" s="33" t="s">
-        <v>40</v>
-      </c>
-      <c r="B86" s="33" t="s">
-        <v>125</v>
+        <v>354</v>
+      </c>
+      <c r="B86" s="44" t="s">
+        <v>115</v>
       </c>
       <c r="C86" s="9" t="s">
-        <v>291</v>
+        <v>276</v>
       </c>
       <c r="G86" s="9" t="s">
-        <v>333</v>
+        <v>318</v>
       </c>
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A87" s="33" t="s">
-        <v>40</v>
-      </c>
-      <c r="B87" s="33" t="s">
-        <v>126</v>
+        <v>354</v>
+      </c>
+      <c r="B87" s="44" t="s">
+        <v>116</v>
       </c>
       <c r="C87" s="9" t="s">
-        <v>292</v>
+        <v>277</v>
       </c>
       <c r="G87" s="9" t="s">
-        <v>333</v>
+        <v>318</v>
       </c>
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A88" s="33" t="s">
-        <v>40</v>
-      </c>
-      <c r="B88" s="33" t="s">
-        <v>127</v>
+        <v>354</v>
+      </c>
+      <c r="B88" s="44" t="s">
+        <v>117</v>
       </c>
       <c r="C88" s="9" t="s">
-        <v>293</v>
+        <v>278</v>
       </c>
       <c r="G88" s="9" t="s">
-        <v>333</v>
+        <v>318</v>
       </c>
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A89" s="33" t="s">
-        <v>40</v>
-      </c>
-      <c r="B89" s="33" t="s">
-        <v>128</v>
+        <v>354</v>
+      </c>
+      <c r="B89" s="44" t="s">
+        <v>118</v>
       </c>
       <c r="C89" s="9" t="s">
-        <v>294</v>
+        <v>279</v>
       </c>
       <c r="G89" s="9" t="s">
-        <v>333</v>
+        <v>318</v>
       </c>
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A90" s="33" t="s">
-        <v>40</v>
-      </c>
-      <c r="B90" s="33" t="s">
-        <v>129</v>
+        <v>354</v>
+      </c>
+      <c r="B90" s="44" t="s">
+        <v>119</v>
       </c>
       <c r="C90" s="9" t="s">
-        <v>295</v>
+        <v>280</v>
       </c>
       <c r="G90" s="9" t="s">
-        <v>333</v>
+        <v>318</v>
       </c>
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A91" s="33" t="s">
-        <v>40</v>
-      </c>
-      <c r="B91" s="33" t="s">
-        <v>130</v>
+        <v>354</v>
+      </c>
+      <c r="B91" s="44" t="s">
+        <v>120</v>
       </c>
       <c r="C91" s="9" t="s">
-        <v>296</v>
+        <v>281</v>
       </c>
       <c r="G91" s="9" t="s">
-        <v>333</v>
+        <v>318</v>
       </c>
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A92" s="33" t="s">
-        <v>40</v>
-      </c>
-      <c r="B92" s="33" t="s">
-        <v>131</v>
+        <v>354</v>
+      </c>
+      <c r="B92" s="44" t="s">
+        <v>121</v>
       </c>
       <c r="C92" s="9" t="s">
-        <v>297</v>
+        <v>282</v>
       </c>
       <c r="G92" s="9" t="s">
-        <v>333</v>
+        <v>318</v>
       </c>
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A93" s="33" t="s">
-        <v>132</v>
+        <v>122</v>
       </c>
     </row>
     <row r="94" spans="1:7" ht="45.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A94" s="33" t="s">
-        <v>139</v>
-      </c>
-      <c r="B94" s="33" t="s">
-        <v>142</v>
+        <v>129</v>
+      </c>
+      <c r="B94" s="44" t="s">
+        <v>362</v>
       </c>
       <c r="C94" s="11" t="s">
-        <v>298</v>
+        <v>283</v>
       </c>
       <c r="G94" s="9" t="s">
-        <v>333</v>
+        <v>318</v>
       </c>
     </row>
     <row r="95" spans="1:7" ht="36" x14ac:dyDescent="0.2">
       <c r="A95" s="33" t="s">
-        <v>139</v>
-      </c>
-      <c r="B95" s="33" t="s">
-        <v>140</v>
+        <v>129</v>
+      </c>
+      <c r="B95" s="44" t="s">
+        <v>363</v>
       </c>
       <c r="C95" s="11" t="s">
-        <v>299</v>
+        <v>284</v>
       </c>
       <c r="G95" s="9" t="s">
-        <v>333</v>
+        <v>318</v>
       </c>
     </row>
     <row r="96" spans="1:7" ht="36" x14ac:dyDescent="0.2">
       <c r="A96" s="33" t="s">
-        <v>139</v>
-      </c>
-      <c r="B96" s="33" t="s">
-        <v>141</v>
+        <v>129</v>
+      </c>
+      <c r="B96" s="44" t="s">
+        <v>130</v>
       </c>
       <c r="C96" s="11" t="s">
-        <v>300</v>
+        <v>285</v>
       </c>
       <c r="G96" s="9" t="s">
-        <v>333</v>
+        <v>318</v>
       </c>
     </row>
     <row r="97" spans="1:8" ht="36" x14ac:dyDescent="0.2">
       <c r="A97" s="33" t="s">
-        <v>146</v>
-      </c>
-      <c r="B97" s="33" t="s">
-        <v>144</v>
+        <v>134</v>
+      </c>
+      <c r="B97" s="44" t="s">
+        <v>132</v>
       </c>
       <c r="C97" s="11" t="s">
-        <v>143</v>
+        <v>131</v>
       </c>
       <c r="G97" s="9" t="s">
-        <v>333</v>
+        <v>318</v>
       </c>
     </row>
     <row r="98" spans="1:8" ht="24" x14ac:dyDescent="0.2">
       <c r="A98" s="33" t="s">
-        <v>149</v>
-      </c>
-      <c r="B98" s="33" t="s">
-        <v>150</v>
+        <v>137</v>
+      </c>
+      <c r="B98" s="44" t="s">
+        <v>138</v>
       </c>
       <c r="C98" s="11" t="s">
-        <v>145</v>
+        <v>133</v>
       </c>
       <c r="G98" s="9" t="s">
-        <v>333</v>
+        <v>318</v>
       </c>
     </row>
     <row r="100" spans="1:8" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
@@ -3503,139 +3495,139 @@
         <v>19</v>
       </c>
       <c r="B100" s="36" t="s">
-        <v>152</v>
+        <v>140</v>
       </c>
       <c r="C100" s="17" t="s">
-        <v>151</v>
+        <v>139</v>
       </c>
     </row>
     <row r="101" spans="1:8" ht="36" x14ac:dyDescent="0.2">
       <c r="A101" s="33" t="s">
-        <v>64</v>
-      </c>
-      <c r="B101" s="33" t="s">
-        <v>154</v>
+        <v>60</v>
+      </c>
+      <c r="B101" s="44" t="s">
+        <v>142</v>
       </c>
       <c r="C101" s="16" t="s">
-        <v>153</v>
+        <v>141</v>
       </c>
       <c r="H101" s="9" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
     </row>
     <row r="102" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A102" s="33" t="s">
-        <v>162</v>
-      </c>
-      <c r="B102" s="33" t="s">
-        <v>242</v>
+        <v>150</v>
+      </c>
+      <c r="B102" s="44" t="s">
+        <v>228</v>
       </c>
       <c r="C102" s="11" t="s">
-        <v>170</v>
+        <v>158</v>
       </c>
     </row>
     <row r="103" spans="1:8" ht="24" x14ac:dyDescent="0.2">
       <c r="A103" s="33" t="s">
-        <v>162</v>
-      </c>
-      <c r="B103" s="33" t="s">
-        <v>155</v>
+        <v>150</v>
+      </c>
+      <c r="B103" s="44" t="s">
+        <v>143</v>
       </c>
       <c r="C103" s="11" t="s">
-        <v>169</v>
+        <v>157</v>
       </c>
     </row>
     <row r="104" spans="1:8" ht="24" x14ac:dyDescent="0.2">
       <c r="A104" s="33" t="s">
-        <v>162</v>
-      </c>
-      <c r="B104" s="33" t="s">
+        <v>150</v>
+      </c>
+      <c r="B104" s="44" t="s">
+        <v>144</v>
+      </c>
+      <c r="C104" s="11" t="s">
         <v>156</v>
-      </c>
-      <c r="C104" s="11" t="s">
-        <v>168</v>
       </c>
     </row>
     <row r="105" spans="1:8" ht="24" x14ac:dyDescent="0.2">
       <c r="A105" s="33" t="s">
-        <v>162</v>
-      </c>
-      <c r="B105" s="33" t="s">
-        <v>157</v>
+        <v>150</v>
+      </c>
+      <c r="B105" s="44" t="s">
+        <v>145</v>
       </c>
       <c r="C105" s="11" t="s">
-        <v>167</v>
+        <v>155</v>
       </c>
     </row>
     <row r="106" spans="1:8" ht="24" x14ac:dyDescent="0.2">
       <c r="A106" s="33" t="s">
-        <v>162</v>
-      </c>
-      <c r="B106" s="33" t="s">
-        <v>159</v>
+        <v>150</v>
+      </c>
+      <c r="B106" s="44" t="s">
+        <v>147</v>
       </c>
       <c r="C106" s="11" t="s">
-        <v>166</v>
+        <v>154</v>
       </c>
     </row>
     <row r="107" spans="1:8" ht="24" x14ac:dyDescent="0.2">
       <c r="A107" s="33" t="s">
-        <v>162</v>
-      </c>
-      <c r="B107" s="33" t="s">
-        <v>158</v>
+        <v>150</v>
+      </c>
+      <c r="B107" s="44" t="s">
+        <v>146</v>
       </c>
       <c r="C107" s="11" t="s">
-        <v>163</v>
+        <v>151</v>
       </c>
     </row>
     <row r="108" spans="1:8" ht="24" x14ac:dyDescent="0.2">
       <c r="A108" s="33" t="s">
-        <v>162</v>
-      </c>
-      <c r="B108" s="33" t="s">
-        <v>243</v>
+        <v>150</v>
+      </c>
+      <c r="B108" s="44" t="s">
+        <v>364</v>
       </c>
       <c r="C108" s="11" t="s">
-        <v>164</v>
+        <v>152</v>
       </c>
     </row>
     <row r="109" spans="1:8" ht="24" x14ac:dyDescent="0.2">
       <c r="A109" s="33" t="s">
-        <v>162</v>
-      </c>
-      <c r="B109" s="33" t="s">
-        <v>160</v>
+        <v>150</v>
+      </c>
+      <c r="B109" s="44" t="s">
+        <v>148</v>
       </c>
       <c r="C109" s="11" t="s">
-        <v>165</v>
+        <v>153</v>
       </c>
     </row>
     <row r="110" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A110" s="33" t="s">
-        <v>132</v>
+        <v>122</v>
       </c>
     </row>
     <row r="112" spans="1:8" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A112" s="37" t="s">
         <v>19</v>
       </c>
-      <c r="B112" s="37" t="s">
-        <v>171</v>
+      <c r="B112" s="46" t="s">
+        <v>159</v>
       </c>
       <c r="C112" s="17" t="s">
-        <v>172</v>
+        <v>160</v>
       </c>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A114" s="33" t="s">
-        <v>69</v>
-      </c>
-      <c r="B114" s="33" t="s">
-        <v>174</v>
+        <v>355</v>
+      </c>
+      <c r="B114" s="44" t="s">
+        <v>162</v>
       </c>
       <c r="C114" s="14" t="s">
-        <v>173</v>
+        <v>161</v>
       </c>
     </row>
   </sheetData>
@@ -3647,10 +3639,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:C126"/>
+  <dimension ref="A1:C127"/>
   <sheetViews>
-    <sheetView topLeftCell="A97" workbookViewId="0">
-      <selection activeCell="C32" sqref="C32"/>
+    <sheetView topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="A35" sqref="A35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3687,1104 +3679,1065 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>347</v>
+        <v>332</v>
       </c>
       <c r="B5">
         <v>1</v>
       </c>
       <c r="C5" s="38" t="s">
-        <v>350</v>
+        <v>335</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>347</v>
+        <v>332</v>
       </c>
       <c r="B6">
         <v>2</v>
       </c>
       <c r="C6" s="24" t="s">
-        <v>348</v>
+        <v>333</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>347</v>
+        <v>332</v>
       </c>
       <c r="B7">
         <v>3</v>
       </c>
       <c r="C7" s="24" t="s">
-        <v>349</v>
+        <v>334</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="9" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>365</v>
+        <v>350</v>
       </c>
       <c r="B9">
         <v>1</v>
       </c>
       <c r="C9" s="39" t="s">
-        <v>351</v>
+        <v>336</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>365</v>
+        <v>350</v>
       </c>
       <c r="B10">
         <v>2</v>
       </c>
       <c r="C10" s="40" t="s">
-        <v>352</v>
+        <v>337</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>365</v>
+        <v>350</v>
       </c>
       <c r="B11">
         <v>3</v>
       </c>
       <c r="C11" s="40" t="s">
-        <v>353</v>
+        <v>338</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>365</v>
+        <v>350</v>
       </c>
       <c r="B12">
         <v>4</v>
       </c>
       <c r="C12" s="40" t="s">
-        <v>354</v>
+        <v>339</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>365</v>
+        <v>350</v>
       </c>
       <c r="B13">
         <v>5</v>
       </c>
       <c r="C13" s="40" t="s">
-        <v>355</v>
+        <v>340</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>365</v>
+        <v>350</v>
       </c>
       <c r="B14">
         <v>6</v>
       </c>
       <c r="C14" s="40" t="s">
-        <v>356</v>
+        <v>341</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>365</v>
+        <v>350</v>
       </c>
       <c r="B15">
         <v>7</v>
       </c>
       <c r="C15" s="40" t="s">
-        <v>357</v>
+        <v>342</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>365</v>
+        <v>350</v>
       </c>
       <c r="B16">
         <v>8</v>
       </c>
       <c r="C16" s="40" t="s">
-        <v>358</v>
+        <v>343</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>365</v>
+        <v>350</v>
       </c>
       <c r="B17">
         <v>9</v>
       </c>
       <c r="C17" s="40" t="s">
-        <v>359</v>
+        <v>344</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>365</v>
+        <v>350</v>
       </c>
       <c r="B18">
         <v>10</v>
       </c>
       <c r="C18" s="40" t="s">
-        <v>360</v>
+        <v>345</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>365</v>
+        <v>350</v>
       </c>
       <c r="B19">
         <v>11</v>
       </c>
       <c r="C19" s="40" t="s">
-        <v>361</v>
+        <v>346</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>365</v>
+        <v>350</v>
       </c>
       <c r="B20">
         <v>12</v>
       </c>
       <c r="C20" s="40" t="s">
-        <v>362</v>
+        <v>347</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>365</v>
+        <v>350</v>
       </c>
       <c r="B21">
         <v>13</v>
       </c>
       <c r="C21" s="40" t="s">
-        <v>363</v>
+        <v>348</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>365</v>
+        <v>350</v>
       </c>
       <c r="B22">
         <v>14</v>
       </c>
       <c r="C22" s="41" t="s">
-        <v>364</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="25" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="C23" s="42"/>
+    </row>
+    <row r="24" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>352</v>
+      </c>
+      <c r="B24" s="2">
+        <v>0</v>
+      </c>
+      <c r="C24" s="24" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>366</v>
-      </c>
-      <c r="B25" s="2">
+        <v>352</v>
+      </c>
+      <c r="B25">
         <v>1</v>
       </c>
       <c r="C25" s="24" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>352</v>
+      </c>
+      <c r="B27" s="2">
+        <v>0</v>
+      </c>
+      <c r="C27" s="24" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>366</v>
-      </c>
-      <c r="B26">
-        <v>2</v>
-      </c>
-      <c r="C26" s="24" t="s">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>352</v>
+      </c>
+      <c r="B28">
+        <v>1</v>
+      </c>
+      <c r="C28" s="24" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>366</v>
-      </c>
-      <c r="B27">
-        <v>8</v>
-      </c>
-      <c r="C27" s="24" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>30</v>
-      </c>
-      <c r="B29" s="2">
+        <v>352</v>
+      </c>
+      <c r="B29">
+        <v>888</v>
+      </c>
+      <c r="C29" s="24" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>353</v>
+      </c>
+      <c r="B32" s="2">
+        <v>0</v>
+      </c>
+      <c r="C32" s="24" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>353</v>
+      </c>
+      <c r="B33">
         <v>1</v>
       </c>
-      <c r="C29" s="24" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>30</v>
-      </c>
-      <c r="B30">
-        <v>2</v>
-      </c>
-      <c r="C30" s="24" t="s">
+      <c r="C33" s="24" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>30</v>
-      </c>
-      <c r="B31">
-        <v>3</v>
-      </c>
-      <c r="C31" s="24" t="s">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>353</v>
+      </c>
+      <c r="B34">
+        <v>888</v>
+      </c>
+      <c r="C34" s="24" t="s">
         <v>28</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>30</v>
-      </c>
-      <c r="B32">
-        <v>4</v>
-      </c>
-      <c r="C32" s="24" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>39</v>
-      </c>
-      <c r="B34" s="2">
-        <v>1</v>
-      </c>
-      <c r="C34" s="24" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>39</v>
+        <v>353</v>
       </c>
       <c r="B35">
-        <v>2</v>
+        <v>8888</v>
       </c>
       <c r="C35" s="24" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
-        <v>39</v>
-      </c>
-      <c r="B36">
-        <v>8</v>
-      </c>
-      <c r="C36" s="24" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>39</v>
-      </c>
-      <c r="B37">
-        <v>9</v>
-      </c>
-      <c r="C37" s="24" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
-        <v>45</v>
-      </c>
-      <c r="B39">
-        <v>4</v>
-      </c>
-      <c r="C39" s="24" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
-        <v>45</v>
-      </c>
-      <c r="B40" s="3">
-        <v>1</v>
-      </c>
-      <c r="C40" s="24" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
-        <v>45</v>
-      </c>
-      <c r="B41">
-        <v>2</v>
-      </c>
-      <c r="C41" s="24" t="s">
-        <v>42</v>
-      </c>
+        <v>27</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B37" s="2"/>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B42">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C42" s="24" t="s">
-        <v>43</v>
+        <v>231</v>
       </c>
     </row>
     <row r="43" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>45</v>
-      </c>
-      <c r="B43">
-        <v>8</v>
-      </c>
-      <c r="C43" s="25" t="s">
-        <v>38</v>
+        <v>42</v>
+      </c>
+      <c r="B43" s="3">
+        <v>1</v>
+      </c>
+      <c r="C43" s="24" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B44">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="C44" s="24" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>42</v>
+      </c>
+      <c r="B45">
+        <v>3</v>
+      </c>
+      <c r="C45" s="24" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>68</v>
+        <v>42</v>
       </c>
       <c r="B46">
-        <v>1</v>
-      </c>
-      <c r="C46" s="24" t="s">
-        <v>25</v>
+        <v>8</v>
+      </c>
+      <c r="C46" s="25" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>68</v>
+        <v>42</v>
       </c>
       <c r="B47">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="C47" s="24" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
-        <v>71</v>
-      </c>
-      <c r="B49">
-        <v>1</v>
-      </c>
-      <c r="C49" s="26" t="s">
-        <v>72</v>
+        <v>35</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="B50">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C50" s="26" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="B51">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C51" s="26" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="B52">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C52" s="26" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="B53">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C53" s="26" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
+        <v>65</v>
+      </c>
+      <c r="B54">
+        <v>888</v>
+      </c>
+      <c r="C54" s="26" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>65</v>
+      </c>
+      <c r="B55">
+        <v>8888</v>
+      </c>
+      <c r="C55" s="4" t="s">
         <v>71</v>
-      </c>
-      <c r="B54">
-        <v>9</v>
-      </c>
-      <c r="C54" s="4" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="57" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A57" t="s">
-        <v>82</v>
-      </c>
-      <c r="B57">
-        <v>1</v>
-      </c>
-      <c r="C57" s="27" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="58" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="B58">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C58" s="27" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
     </row>
     <row r="59" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="B59">
+        <v>2</v>
+      </c>
+      <c r="C59" s="27" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>76</v>
+      </c>
+      <c r="B60">
         <v>3</v>
       </c>
-      <c r="C59" s="25" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="61" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A61" t="s">
-        <v>94</v>
-      </c>
-      <c r="B61">
-        <v>1</v>
-      </c>
-      <c r="C61" s="28" t="s">
-        <v>301</v>
+      <c r="C60" s="25" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="62" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>94</v>
+        <v>87</v>
       </c>
       <c r="B62">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C62" s="28" t="s">
-        <v>302</v>
+        <v>286</v>
       </c>
     </row>
     <row r="63" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>94</v>
+        <v>87</v>
       </c>
       <c r="B63">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C63" s="28" t="s">
-        <v>303</v>
+        <v>287</v>
       </c>
     </row>
     <row r="64" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>94</v>
+        <v>87</v>
       </c>
       <c r="B64">
+        <v>3</v>
+      </c>
+      <c r="C64" s="28" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>87</v>
+      </c>
+      <c r="B65">
         <v>4</v>
       </c>
-      <c r="C64" s="28" t="s">
-        <v>304</v>
-      </c>
-    </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A65" t="s">
-        <v>94</v>
-      </c>
-      <c r="B65">
-        <v>8</v>
-      </c>
-      <c r="C65" s="29" t="s">
-        <v>305</v>
+      <c r="C65" s="28" t="s">
+        <v>289</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>94</v>
+        <v>87</v>
       </c>
       <c r="B66">
+        <v>8</v>
+      </c>
+      <c r="C66" s="29" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>87</v>
+      </c>
+      <c r="B67">
         <v>9</v>
       </c>
-      <c r="C66" s="29" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="68" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A68" t="s">
-        <v>100</v>
-      </c>
-      <c r="B68">
-        <v>1</v>
-      </c>
-      <c r="C68" s="27" t="s">
-        <v>306</v>
+      <c r="C67" s="29" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="69" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
       <c r="B69">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C69" s="27" t="s">
-        <v>307</v>
+        <v>291</v>
       </c>
     </row>
     <row r="70" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
       <c r="B70">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C70" s="27" t="s">
-        <v>308</v>
+        <v>292</v>
       </c>
     </row>
     <row r="71" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
       <c r="B71">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="C71" s="27" t="s">
-        <v>38</v>
+        <v>293</v>
       </c>
     </row>
     <row r="72" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
       <c r="B72">
+        <v>8</v>
+      </c>
+      <c r="C72" s="27" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>93</v>
+      </c>
+      <c r="B73">
         <v>9</v>
       </c>
-      <c r="C72" s="25" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="76" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A76" t="s">
-        <v>109</v>
-      </c>
-      <c r="B76">
-        <v>1</v>
-      </c>
-      <c r="C76" s="27" t="s">
-        <v>104</v>
+      <c r="C73" s="25" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="77" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
       <c r="B77">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C77" s="27" t="s">
-        <v>105</v>
+        <v>97</v>
       </c>
     </row>
     <row r="78" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
       <c r="B78">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C78" s="27" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
     </row>
     <row r="79" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
       <c r="B79">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C79" s="27" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
     </row>
     <row r="80" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
       <c r="B80">
+        <v>4</v>
+      </c>
+      <c r="C80" s="27" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>102</v>
+      </c>
+      <c r="B81">
         <v>8</v>
       </c>
-      <c r="C80" s="25" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A81" t="s">
-        <v>109</v>
-      </c>
-      <c r="B81">
+      <c r="C81" s="25" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>102</v>
+      </c>
+      <c r="B82">
         <v>9</v>
       </c>
-      <c r="C81" s="24" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A83" t="s">
-        <v>119</v>
-      </c>
-      <c r="B83">
-        <v>1</v>
-      </c>
-      <c r="C83" s="24" t="s">
-        <v>309</v>
+      <c r="C82" s="24" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
       <c r="B84">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C84" s="24" t="s">
-        <v>310</v>
+        <v>294</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
       <c r="B85">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C85" s="24" t="s">
-        <v>311</v>
+        <v>295</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
       <c r="B86">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C86" s="24" t="s">
-        <v>312</v>
+        <v>296</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
       <c r="B87">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C87" s="24" t="s">
-        <v>332</v>
+        <v>297</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
       <c r="B88">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C88" s="24" t="s">
-        <v>331</v>
+        <v>317</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
       <c r="B89">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C89" s="24" t="s">
-        <v>313</v>
+        <v>316</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
       <c r="B90">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C90" s="24" t="s">
-        <v>314</v>
+        <v>298</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
       <c r="B91">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C91" s="24" t="s">
-        <v>315</v>
+        <v>299</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
       <c r="B92">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C92" s="24" t="s">
-        <v>316</v>
+        <v>300</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
       <c r="B93">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C93" s="24" t="s">
-        <v>317</v>
+        <v>301</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
       <c r="B94">
+        <v>11</v>
+      </c>
+      <c r="C94" s="24" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
+        <v>112</v>
+      </c>
+      <c r="B95">
         <v>12</v>
       </c>
-      <c r="C94" s="24" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="96" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A96" t="s">
-        <v>138</v>
-      </c>
-      <c r="B96">
-        <v>1</v>
-      </c>
-      <c r="C96" s="27" t="s">
-        <v>133</v>
+      <c r="C95" s="24" t="s">
+        <v>303</v>
       </c>
     </row>
     <row r="97" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>138</v>
+        <v>128</v>
       </c>
       <c r="B97">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C97" s="27" t="s">
-        <v>134</v>
+        <v>123</v>
       </c>
     </row>
     <row r="98" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>138</v>
+        <v>128</v>
       </c>
       <c r="B98">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C98" s="27" t="s">
-        <v>135</v>
+        <v>124</v>
       </c>
     </row>
     <row r="99" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>138</v>
+        <v>128</v>
       </c>
       <c r="B99">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C99" s="27" t="s">
-        <v>136</v>
+        <v>125</v>
       </c>
     </row>
     <row r="100" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>138</v>
+        <v>128</v>
       </c>
       <c r="B100">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C100" s="27" t="s">
-        <v>137</v>
+        <v>126</v>
       </c>
     </row>
     <row r="101" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>138</v>
+        <v>128</v>
       </c>
       <c r="B101">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C101" s="27" t="s">
-        <v>76</v>
+        <v>127</v>
       </c>
     </row>
     <row r="102" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>138</v>
+        <v>128</v>
       </c>
       <c r="B102">
+        <v>8</v>
+      </c>
+      <c r="C102" s="27" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A103" t="s">
+        <v>128</v>
+      </c>
+      <c r="B103">
         <v>9</v>
       </c>
-      <c r="C102" s="25" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="104" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A104" t="s">
-        <v>147</v>
-      </c>
-      <c r="B104">
-        <v>1</v>
-      </c>
-      <c r="C104" s="25" t="s">
-        <v>319</v>
+      <c r="C103" s="25" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="105" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>147</v>
+        <v>135</v>
       </c>
       <c r="B105">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C105" s="25" t="s">
-        <v>320</v>
+        <v>304</v>
       </c>
     </row>
     <row r="106" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>147</v>
+        <v>135</v>
       </c>
       <c r="B106">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C106" s="25" t="s">
-        <v>321</v>
+        <v>305</v>
       </c>
     </row>
     <row r="107" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>147</v>
+        <v>135</v>
       </c>
       <c r="B107">
+        <v>3</v>
+      </c>
+      <c r="C107" s="25" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="108" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A108" t="s">
+        <v>135</v>
+      </c>
+      <c r="B108">
         <v>4</v>
       </c>
-      <c r="C107" s="25" t="s">
-        <v>322</v>
-      </c>
-    </row>
-    <row r="109" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A109" t="s">
-        <v>148</v>
-      </c>
-      <c r="B109">
-        <v>1</v>
-      </c>
-      <c r="C109" s="25" t="s">
-        <v>323</v>
+      <c r="C108" s="25" t="s">
+        <v>307</v>
       </c>
     </row>
     <row r="110" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>148</v>
+        <v>136</v>
       </c>
       <c r="B110">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C110" s="25" t="s">
-        <v>324</v>
+        <v>308</v>
       </c>
     </row>
     <row r="111" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>148</v>
+        <v>136</v>
       </c>
       <c r="B111">
+        <v>2</v>
+      </c>
+      <c r="C111" s="25" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="112" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A112" t="s">
+        <v>136</v>
+      </c>
+      <c r="B112">
         <v>3</v>
       </c>
-      <c r="C111" s="25" t="s">
-        <v>325</v>
-      </c>
-    </row>
-    <row r="113" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A113" t="s">
-        <v>161</v>
-      </c>
-      <c r="B113">
+      <c r="C112" s="25" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="114" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A114" t="s">
+        <v>149</v>
+      </c>
+      <c r="B114">
         <v>1</v>
       </c>
-      <c r="C113" s="25" t="s">
-        <v>330</v>
-      </c>
-    </row>
-    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A114" t="s">
-        <v>161</v>
-      </c>
-      <c r="B114">
-        <v>2</v>
-      </c>
-      <c r="C114" s="24" t="s">
-        <v>326</v>
+      <c r="C114" s="25" t="s">
+        <v>315</v>
       </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>161</v>
+        <v>149</v>
       </c>
       <c r="B115">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C115" s="24" t="s">
-        <v>327</v>
+        <v>311</v>
       </c>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>161</v>
+        <v>149</v>
       </c>
       <c r="B116">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C116" s="24" t="s">
-        <v>328</v>
+        <v>312</v>
       </c>
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>161</v>
+        <v>149</v>
       </c>
       <c r="B117">
+        <v>4</v>
+      </c>
+      <c r="C117" s="24" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="118" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A118" t="s">
+        <v>149</v>
+      </c>
+      <c r="B118">
         <v>5</v>
       </c>
-      <c r="C117" s="24" t="s">
-        <v>329</v>
-      </c>
-    </row>
-    <row r="120" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A120" t="s">
-        <v>336</v>
-      </c>
-      <c r="B120">
-        <v>1</v>
-      </c>
-      <c r="C120" t="s">
-        <v>341</v>
+      <c r="C118" s="24" t="s">
+        <v>314</v>
       </c>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>336</v>
+        <v>321</v>
       </c>
       <c r="B121">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C121" t="s">
-        <v>340</v>
+        <v>326</v>
       </c>
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>336</v>
+        <v>321</v>
       </c>
       <c r="B122">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C122" t="s">
-        <v>342</v>
+        <v>325</v>
       </c>
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>336</v>
+        <v>321</v>
       </c>
       <c r="B123">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C123" t="s">
-        <v>339</v>
+        <v>327</v>
       </c>
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>336</v>
+        <v>321</v>
       </c>
       <c r="B124">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C124" t="s">
-        <v>343</v>
+        <v>324</v>
       </c>
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>336</v>
+        <v>321</v>
       </c>
       <c r="B125">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C125" t="s">
-        <v>337</v>
+        <v>328</v>
       </c>
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>336</v>
+        <v>321</v>
       </c>
       <c r="B126">
+        <v>6</v>
+      </c>
+      <c r="C126" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="127" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A127" t="s">
+        <v>321</v>
+      </c>
+      <c r="B127">
         <v>7</v>
       </c>
-      <c r="C126" t="s">
-        <v>344</v>
+      <c r="C127" t="s">
+        <v>329</v>
       </c>
     </row>
   </sheetData>

</xml_diff>